<commit_message>
Removed the 0.8V Reference circuit, changed the opamp, and changed the testpoints to make testing easier. Not sure how the connector is meant to be set up though
</commit_message>
<xml_diff>
--- a/ActivePrechargeBOM.csv.xlsx
+++ b/ActivePrechargeBOM.csv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gavin\Documents\LHRs GitHub\PS-ActivePrecharge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A12A9AA8-A320-49DB-94AE-67C10D1167D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2004387C-B08D-4134-B424-4D0E5001FA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13E35209-BEF2-4DE5-ADBC-E5DDA57B7207}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{13E35209-BEF2-4DE5-ADBC-E5DDA57B7207}"/>
   </bookViews>
   <sheets>
     <sheet name="ActivePrechargeBOM" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +541,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -704,8 +722,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,7 +1105,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1153,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -1146,7 +1167,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -1160,7 +1181,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>9</v>
       </c>
       <c r="B6" t="s">
@@ -1188,7 +1209,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1202,7 +1223,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9" t="s">
@@ -1230,7 +1251,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -1244,7 +1265,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1258,7 +1279,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>5</v>
       </c>
       <c r="B13" t="s">
@@ -1272,7 +1293,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" t="s">
@@ -1286,7 +1307,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>5</v>
       </c>
       <c r="B15" t="s">
@@ -1300,7 +1321,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>1</v>
       </c>
       <c r="B16" t="s">
@@ -1314,7 +1335,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
       <c r="B17" t="s">
@@ -1469,5 +1490,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>